<commit_message>
Adding queries for Neo. Changes to format of RDF spreadsheet. Updates to instructions and model.
</commit_message>
<xml_diff>
--- a/Annual2017-EU/data/Neo4jModel.xlsx
+++ b/Annual2017-EU/data/Neo4jModel.xlsx
@@ -50,15 +50,9 @@
     <t>participatesIn</t>
   </si>
   <si>
-    <t>Node1</t>
-  </si>
-  <si>
     <t>Relation</t>
   </si>
   <si>
-    <t>Node2</t>
-  </si>
-  <si>
     <t>Treat1</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>Phase 2 Double-blind study of Serum 114</t>
   </si>
   <si>
-    <t>treatment</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -92,10 +83,19 @@
     <t>Relations</t>
   </si>
   <si>
-    <t>Node Parameter:Value Pairs</t>
-  </si>
-  <si>
     <t>Property</t>
+  </si>
+  <si>
+    <t>StartNode</t>
+  </si>
+  <si>
+    <t>EndNode</t>
+  </si>
+  <si>
+    <t>Node PV</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
@@ -167,12 +167,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -180,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,16 +211,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -228,15 +226,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -558,119 +558,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
     <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.26953125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="E4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="G4" s="12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="B5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" s="5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="E6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -678,14 +680,14 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="E7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>19</v>
+      <c r="E7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -693,112 +695,132 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
formatting and protection changes
</commit_message>
<xml_diff>
--- a/Annual2017-EU/data/Neo4jModel.xlsx
+++ b/Annual2017-EU/data/Neo4jModel.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
-  <si>
-    <t>hasTreatment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Person1</t>
   </si>
@@ -44,12 +41,6 @@
     <t>Bob</t>
   </si>
   <si>
-    <t>hasTreatmentArm</t>
-  </si>
-  <si>
-    <t>participatesIn</t>
-  </si>
-  <si>
     <t>Relation</t>
   </si>
   <si>
@@ -96,6 +87,48 @@
   </si>
   <si>
     <t>Table 2: Node P:V Pairs</t>
+  </si>
+  <si>
+    <t>enrolledIn</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>treatmentArm</t>
+  </si>
+  <si>
+    <t>Person2</t>
+  </si>
+  <si>
+    <t>Treat2</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>Protocol1</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>Phase 2 Trial of Serum 114 in patients with acute episodes of ultraviolence</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>50 mg Serum 114</t>
   </si>
 </sst>
 </file>
@@ -205,24 +238,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -245,7 +262,34 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,284 +610,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="10"/>
+    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="15" width="8.7265625" style="10"/>
+    <col min="16" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="E1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="18">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="C5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G6" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="G9" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="G10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="snrz2gZuCzal77TQGrz4Kj59YDl2Gt2i5kWDrHwExEEQQq5F2Kr1JIeCtrpLoFcG8wwErH0/clfxpUqrd0Q95g==" saltValue="7Nnq91TzhbzxM8sM/lNWmQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WKNUlCgGBJLyr6A+kcOmcQaM8b4zmrsCQpdFWjvHYthwEigpGp3gT8GybAG/4NdfGy7mM7dE/m7WpbAtsU6vwA==" saltValue="6s2RvyhrKymoP9YMki8inA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
push for use on server
</commit_message>
<xml_diff>
--- a/Annual2017-EU/data/Neo4jModel.xlsx
+++ b/Annual2017-EU/data/Neo4jModel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Person1</t>
   </si>
@@ -83,9 +83,6 @@
     <t>label</t>
   </si>
   <si>
-    <t>Table 1. Relations</t>
-  </si>
-  <si>
     <t>Table 2: Node P:V Pairs</t>
   </si>
   <si>
@@ -98,37 +95,7 @@
     <t>treatmentArm</t>
   </si>
   <si>
-    <t>Person2</t>
-  </si>
-  <si>
-    <t>Treat2</t>
-  </si>
-  <si>
-    <t>protocol</t>
-  </si>
-  <si>
-    <t>Protocol1</t>
-  </si>
-  <si>
-    <t>phase</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>Phase 2 Trial of Serum 114 in patients with acute episodes of ultraviolence</t>
-  </si>
-  <si>
-    <t>Sally</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>50 mg Serum 114</t>
+    <t>Table 1. Nodes and Relations</t>
   </si>
 </sst>
 </file>
@@ -613,7 +580,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -631,12 +598,12 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
       <c r="E1" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="15"/>
@@ -666,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>1</v>
@@ -686,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>5</v>
@@ -706,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>5</v>
@@ -722,15 +689,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="E6" s="14" t="s">
         <v>5</v>
       </c>
@@ -742,15 +703,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="E7" s="14" t="s">
         <v>5</v>
       </c>
@@ -762,86 +717,44 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
@@ -958,7 +871,6 @@
       <c r="G27" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="WKNUlCgGBJLyr6A+kcOmcQaM8b4zmrsCQpdFWjvHYthwEigpGp3gT8GybAG/4NdfGy7mM7dE/m7WpbAtsU6vwA==" saltValue="6s2RvyhrKymoP9YMki8inA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Changing to caps on Nodes, etc.
</commit_message>
<xml_diff>
--- a/Annual2017-EU/data/Neo4jModel.xlsx
+++ b/Annual2017-EU/data/Neo4jModel.xlsx
@@ -29,12 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
-    <t>Person1</t>
-  </si>
-  <si>
-    <t>Study1</t>
-  </si>
-  <si>
     <t>Placebo</t>
   </si>
   <si>
@@ -44,18 +38,12 @@
     <t>Relation</t>
   </si>
   <si>
-    <t>Treat1</t>
-  </si>
-  <si>
     <t>Node</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
@@ -86,16 +74,28 @@
     <t>Table 2: Node P:V Pairs</t>
   </si>
   <si>
-    <t>enrolledIn</t>
-  </si>
-  <si>
     <t>treatment</t>
   </si>
   <si>
-    <t>treatmentArm</t>
-  </si>
-  <si>
     <t>Table 1. Nodes and Relations</t>
+  </si>
+  <si>
+    <t>PERSON1</t>
+  </si>
+  <si>
+    <t>STUDY1</t>
+  </si>
+  <si>
+    <t>TREAT1</t>
+  </si>
+  <si>
+    <t>enrolledin</t>
+  </si>
+  <si>
+    <t>treatmentarm</t>
+  </si>
+  <si>
+    <t>firstname</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,71 +598,71 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
       <c r="E1" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>5</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>9</v>
       </c>
       <c r="G4" s="18">
         <v>32</v>
@@ -670,22 +670,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -693,13 +693,13 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="E6" s="14" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -707,13 +707,13 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="E7" s="14" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -871,6 +871,7 @@
       <c r="G27" s="7"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="uEaKpTMGjruOQ15W5MQZzWb6/1SH3DEjFFMu3ieh11ApvAyvfqtLFxroLJHhI5i7bNFgV/F2zql4yZKmK49K/g==" saltValue="LeCwevEdRqmgO/9ncoAxkQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>